<commit_message>
Added a test case on CreateAccount methods. Which has to throw an exception if you asked for an account other than the Chequings or Savings.
</commit_message>
<xml_diff>
--- a/doc/Test cases.xlsx
+++ b/doc/Test cases.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="87">
   <si>
     <t>Expected Result</t>
   </si>
@@ -268,6 +268,27 @@
   </si>
   <si>
     <t>Sanjay Sohal</t>
+  </si>
+  <si>
+    <t>Verifies that there are only two type of account allowed</t>
+  </si>
+  <si>
+    <t>1. Call the createAcc account parameters for accountType, owner respectively</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Throws an exception saying that invalid type of account provided </t>
+  </si>
+  <si>
+    <t>1. Throws an exception which states, invald type of account provided</t>
+  </si>
+  <si>
+    <t>CreateAccount class method</t>
+  </si>
+  <si>
+    <t>TC007</t>
+  </si>
+  <si>
+    <t>1. Accounttype: student                  2. Accountname: John</t>
   </si>
 </sst>
 </file>
@@ -603,7 +624,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -763,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="I8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1136,8 +1157,55 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15.75" thickBot="1">
-      <c r="E8" s="2"/>
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="84.75" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M8" s="3">
+        <v>42107</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O8" s="3">
+        <v>42107</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Split the creation of Savings and Chequing into different test cases
</commit_message>
<xml_diff>
--- a/doc/Test cases.xlsx
+++ b/doc/Test cases.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="93">
   <si>
     <t>Expected Result</t>
   </si>
@@ -186,24 +186,9 @@
     <t>TC003</t>
   </si>
   <si>
-    <t>Verify that an account can be created for either Savings or Chequing</t>
-  </si>
-  <si>
-    <t>1. User knows what kind of account they want to createq</t>
-  </si>
-  <si>
-    <t>1. A New Savings Account object is created.                   2. A New Chequings Account object Is created.</t>
-  </si>
-  <si>
     <t>Create Accounts Test Case</t>
   </si>
   <si>
-    <t>1. If a Savings Account is created, a message saying a Savings Account has been created should display.                                                                        2. If a Chequings Account is created, a message saying a Chequings Account has been created should display.</t>
-  </si>
-  <si>
-    <t>1. If Savings or Chequing is inserted for card type, the result is as specified.                           2. If a user doesn’t enter one of these two accounts, an error message telling them that type of account doesn’t exist will be displayed.</t>
-  </si>
-  <si>
     <t>TC004</t>
   </si>
   <si>
@@ -237,9 +222,6 @@
     <t>1. If the deposit is successful, a message letting you know that you have deposited the amount should be seen.                                                           2. If you enter a number less or equal to zero, an error message will be displayed.</t>
   </si>
   <si>
-    <t>1. Create a Savings Account using the createAcc() method of CreateAccount class                                                         2. Create a Chequing Account using the createAcc() method of CreateAccount class</t>
-  </si>
-  <si>
     <t>1. If the withdrawl is made successfully, the balance should be equal to 23 and no error message displayed.                                             2. If the withdrawl is unsuccessful, the user is notified of the mistake in balance.</t>
   </si>
   <si>
@@ -289,6 +271,42 @@
   </si>
   <si>
     <t>1. Accounttype: student                  2. Accountname: John</t>
+  </si>
+  <si>
+    <t>Verify that an account can be created for Savings</t>
+  </si>
+  <si>
+    <t>Verify that an account can be created for Chequing</t>
+  </si>
+  <si>
+    <t>1. User knows what kind of account they want to create</t>
+  </si>
+  <si>
+    <t>1. Create a Savings Account using the createAcc() method of CreateAccount class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                        1. Create a Chequing Account using the createAcc() method of CreateAccount class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A New Savings Account object is created.                   </t>
+  </si>
+  <si>
+    <t>1. A New Chequings Account object Is created.</t>
+  </si>
+  <si>
+    <t>1. If a Savings Account is created, a message saying a Savings Account has been created should display.</t>
+  </si>
+  <si>
+    <t>1. If a Chequings Account is created, a message saying a Chequings Account has been created should display.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. If Savings is inserted for card type, the result is as specified.                           </t>
+  </si>
+  <si>
+    <t>1. If Chequing is inserted for card type, the result is as specified.</t>
+  </si>
+  <si>
+    <t>TC008</t>
   </si>
 </sst>
 </file>
@@ -624,7 +642,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -782,10 +800,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -957,7 +975,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="105">
+    <row r="4" spans="1:16" ht="60">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -965,31 +983,31 @@
         <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
         <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>49</v>
@@ -1007,39 +1025,39 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="90">
+    <row r="5" spans="1:16" ht="60">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>49</v>
@@ -1057,39 +1075,39 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="120">
+    <row r="6" spans="1:16" ht="90">
       <c r="A6" t="s">
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
         <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>49</v>
@@ -1107,103 +1125,153 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" ht="135">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:16" ht="120">
+      <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>72</v>
+      <c r="B7" t="s">
+        <v>66</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M7" s="3">
-        <v>42087</v>
+        <v>49</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="O7" s="3">
-        <v>42109</v>
+        <v>49</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" ht="84.75" customHeight="1">
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="135">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="M8" s="3">
+        <v>42087</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O8" s="3">
+        <v>42109</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="1" customFormat="1" ht="84.75" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M9" s="3">
         <v>42107</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="O8" s="3">
+      <c r="N9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O9" s="3">
         <v>42107</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Split the CreateCard test cases into 3, debit, credit, and exception. Added an else statement in CreateCard which returns exception if wrong type of card inputed. We now have 10 Test Cases ! ! !
</commit_message>
<xml_diff>
--- a/doc/Test cases.xlsx
+++ b/doc/Test cases.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="105">
   <si>
     <t>Expected Result</t>
   </si>
@@ -156,24 +156,9 @@
     <t>TC002</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that the CreateCard class creates both a Debit and Credit Card.  </t>
-  </si>
-  <si>
     <t>1. User knows what kind of Card they want to create.</t>
   </si>
   <si>
-    <t>1. First Create a Instance of a Card.          2. Create a Debit Card using the instance.                                                     3. Create a Credit Card using the same instance.</t>
-  </si>
-  <si>
-    <t>1. New DebitCard object with name Tyler Test                 2. New CreditCard object with name Tyler Test</t>
-  </si>
-  <si>
-    <t>1. First created was the Debit Card so a message that A Debit Card has been created should show.     2. The Credit Card is created after and a message that A Credit Card has been created should be displayed.</t>
-  </si>
-  <si>
-    <t>1. If the type of card is correctly input, the result should be as expected.                             2. If a type of card does not exist, an error message is displayed saying card cannot be created.</t>
-  </si>
-  <si>
     <t>Create Card Test Case</t>
   </si>
   <si>
@@ -307,6 +292,57 @@
   </si>
   <si>
     <t>TC008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the CreateCard class creates a Debit Card.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the CreateCard class creates a Credit Card.  </t>
+  </si>
+  <si>
+    <t>1. First Create a Instance of a Card.          2. Create a Debit Card using the instance.</t>
+  </si>
+  <si>
+    <t>1. First Create a Instance of a Card.                                                          2. Create a Credit Card using the same instance.</t>
+  </si>
+  <si>
+    <t>1. New DebitCard object with name Tyler Test</t>
+  </si>
+  <si>
+    <t>1. New CreditCard object with name Tyler Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Creates the Debit Card so a message that "A Debit Card has been created" should show.     </t>
+  </si>
+  <si>
+    <t>1. The Credit Card is created and a message that "A Credit Card has been created" should be displayed.</t>
+  </si>
+  <si>
+    <t>1. If the type of card is Debit, the result should be as expected.</t>
+  </si>
+  <si>
+    <t>1. If the type of card is Credit, the result should be as expected.</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>1. First Create a Instance of a Card.                                                          2. Tries to create a "Rewards" Card using the same instance.</t>
+  </si>
+  <si>
+    <t>1. New "Rewards" card object with name WrongCard Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Throws an exception saying that invalid type of card provided </t>
+  </si>
+  <si>
+    <t>1. Throws an exception which states, invald type of card provided</t>
+  </si>
+  <si>
+    <t>TC009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the CreateCard method only creates either a Credit or a Debit Card.  </t>
   </si>
 </sst>
 </file>
@@ -642,7 +678,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -800,10 +836,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -925,7 +961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="90">
+    <row r="3" spans="1:16" ht="60">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -933,40 +969,40 @@
         <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
         <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>31</v>
@@ -980,43 +1016,43 @@
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
         <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>31</v>
@@ -1030,43 +1066,43 @@
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>31</v>
@@ -1075,48 +1111,48 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="90">
+    <row r="6" spans="1:16" ht="60">
       <c r="A6" t="s">
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
         <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>31</v>
@@ -1125,48 +1161,48 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="120">
+    <row r="7" spans="1:16" ht="90">
       <c r="A7" t="s">
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>31</v>
@@ -1175,103 +1211,203 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" ht="135">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:16" ht="120">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>79</v>
+      <c r="B8" t="s">
+        <v>74</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="M8" s="3">
-        <v>42087</v>
+        <v>44</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O8" s="3">
-        <v>42109</v>
+        <v>44</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" ht="84.75" customHeight="1">
+    <row r="9" spans="1:16" s="1" customFormat="1" ht="135">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="L9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M9" s="3">
+        <v>42087</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O9" s="3">
+        <v>42109</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="84.75" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="M9" s="3">
+      <c r="L10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M10" s="3">
+        <v>42087</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O10" s="3">
         <v>42107</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O9" s="3">
+      <c r="P10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="90">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M11" s="3">
+        <v>42087</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O11" s="3">
         <v>42107</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P11" s="1" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>